<commit_message>
integrate backend service initialization
</commit_message>
<xml_diff>
--- a/ExcelAddIn/Sample_Financial_Data.xlsx
+++ b/ExcelAddIn/Sample_Financial_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qianf\OneDrive\桌面\project\ExcelAddIn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\ExcelAddIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7A4ECF-83A2-4215-8544-AA77752F6B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF0C0CB-944D-439F-8A13-DC5AC5DA30FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialData" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -162,7 +162,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -468,12 +468,12 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -519,7 +519,7 @@
         <v>2493388</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -542,7 +542,7 @@
         <v>2444103</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -565,7 +565,7 @@
         <v>1514060</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -588,7 +588,7 @@
         <v>4358031</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -611,7 +611,7 @@
         <v>4053205</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -634,7 +634,7 @@
         <v>1604299</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -657,7 +657,7 @@
         <v>1741633</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -680,7 +680,7 @@
         <v>1282839</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -703,7 +703,7 @@
         <v>1820555</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -738,12 +738,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="31.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -754,7 +754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -765,7 +765,7 @@
         <v>302.45999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -776,7 +776,7 @@
         <v>228.46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -787,7 +787,7 @@
         <v>58.99</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -810,13 +810,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.23046875" customWidth="1"/>
+    <col min="3" max="3" width="24.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +827,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45809</v>
       </c>
@@ -838,7 +838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45809</v>
       </c>
@@ -849,7 +849,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45809</v>
       </c>
@@ -860,7 +860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45809</v>
       </c>
@@ -871,7 +871,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45810</v>
       </c>
@@ -882,7 +882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45810</v>
       </c>
@@ -893,7 +893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45810</v>
       </c>
@@ -904,7 +904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45810</v>
       </c>
@@ -915,7 +915,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45811</v>
       </c>
@@ -926,7 +926,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45811</v>
       </c>
@@ -937,7 +937,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45811</v>
       </c>
@@ -948,7 +948,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45811</v>
       </c>

</xml_diff>